<commit_message>
refactor group exporter, add attribute selector for group exporter
</commit_message>
<xml_diff>
--- a/web/templates/group.xlsx
+++ b/web/templates/group.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenceslaus/PhpstormProjects/arina/web/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18780E4E-8B42-3A45-A7AA-E4F63E8A6251}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8A9FCCA7-0A0E-3443-BDF3-1C23F478BE43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23360" windowHeight="12980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>№ п/п</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Прізвище, ім'я, по батькові студента</t>
-  </si>
-  <si>
-    <t>Бюджет/контракт</t>
   </si>
   <si>
     <t>Список студентів групи</t>
@@ -39,13 +33,16 @@
   <si>
     <t>Староста</t>
   </si>
+  <si>
+    <t>№</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -121,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -156,13 +153,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -171,76 +190,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -250,13 +203,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -265,38 +214,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -305,11 +250,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -320,16 +262,16 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,32 +279,19 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,179 +572,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="178" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="178" zoomScaleNormal="100" zoomScaleSheetLayoutView="178" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" customWidth="1"/>
-    <col min="5" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="0.1640625" customWidth="1"/>
-    <col min="11" max="256" width="8.83203125" customWidth="1"/>
+    <col min="5" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="3.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="0.1640625" customWidth="1"/>
+    <col min="12" max="257" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="18">
-      <c r="B1" s="21" t="s">
+    <row r="1" spans="2:20" ht="18">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="2:20" ht="18" customHeight="1">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="2:20" ht="18" customHeight="1" thickBot="1">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" ht="20" customHeight="1">
+      <c r="B4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="2:20" ht="15" customHeight="1">
+      <c r="B5" s="21">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="2:20" ht="15" customHeight="1" thickBot="1">
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="C8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="2:20" ht="14.25" customHeight="1"/>
+    <row r="10" spans="2:20">
+      <c r="C10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
     </row>
-    <row r="2" spans="2:19" ht="18">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="2:19" ht="20" thickBot="1">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="2:19" ht="15" customHeight="1">
-      <c r="B4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="2:19">
-      <c r="B5" s="24"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="2:19" ht="78" customHeight="1">
-      <c r="B6" s="25"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="27"/>
-    </row>
-    <row r="7" spans="2:19" ht="16">
-      <c r="B7" s="10">
-        <v>1</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="2:19" ht="17" thickBot="1">
-      <c r="B8" s="12"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="2:19" ht="14.25" customHeight="1"/>
-    <row r="10" spans="2:19">
-      <c r="C10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:19" ht="9" customHeight="1"/>
-    <row r="12" spans="2:19">
-      <c r="C12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14"/>
-    </row>
+    <row r="11" spans="2:20" ht="9" customHeight="1"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C4:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="C4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294"/>

</xml_diff>